<commit_message>
json estructura persona funcionando
</commit_message>
<xml_diff>
--- a/RemuneracionesPT/uploads/reliquidaciones/part-time/reliquida-partime.xlsx
+++ b/RemuneracionesPT/uploads/reliquidaciones/part-time/reliquida-partime.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>C.COSTO</t>
   </si>
@@ -70,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +201,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -547,8 +555,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -870,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,6 +1028,40 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>4.5</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
añade local storage a los proceso
</commit_message>
<xml_diff>
--- a/RemuneracionesPT/uploads/reliquidaciones/part-time/reliquida-partime.xlsx
+++ b/RemuneracionesPT/uploads/reliquidaciones/part-time/reliquida-partime.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>C.COSTO</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>JUZPTPT104</t>
+  </si>
+  <si>
+    <t>juzpassa</t>
+  </si>
+  <si>
+    <t>jejeje</t>
+  </si>
+  <si>
+    <t>pepe</t>
   </si>
 </sst>
 </file>
@@ -879,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,6 +1071,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>